<commit_message>
début documentation livrable 2
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adminesp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adminesp\Documents\Project-ESP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -51,51 +51,12 @@
     <t>c</t>
   </si>
   <si>
-    <t>En tant que administrateur, je souhaite pouvoir avoir des niveaux de droits d'accès différents afin de pouvoir avoir des droits sur différentes section du site.</t>
-  </si>
-  <si>
-    <t>Un administrateur qui n'a pas le droit d'accès ne peut modifier une page.</t>
-  </si>
-  <si>
     <t>La connection se fait avec un email et un mot de passe.</t>
   </si>
   <si>
     <t>Il devient impossible d'effectuer une connexion si l'administrateur est déjà connecté.</t>
   </si>
   <si>
-    <t>En tant que super administrateur, je souhaite pourvoir inscrire un nouvel administrateur afin de pouvoir donné accès à un nouveau membre.</t>
-  </si>
-  <si>
-    <t>Seul le super administrateur peut effectué des inscriptions.</t>
-  </si>
-  <si>
-    <t>En tant que administrateur, je souhaire pouvoir modifier les sections du sites auquel j'ai accès afin de maintenir le site à jour.</t>
-  </si>
-  <si>
-    <t>L'administrateur ne peut modifier une section auquel il n'a pas accès.</t>
-  </si>
-  <si>
-    <t>En tant que super administrateur, je souhaite recevoir des notifications lorsque les administrateur font des changements au site afin de valider ceux-ci.</t>
-  </si>
-  <si>
-    <t>La notification indique la section qui a été modifié ainsi que l'admin qui l'a effectué.</t>
-  </si>
-  <si>
-    <t>En tant que super administrateur, je souhaite pourvoir changer les droits des administrateurs afin de choisir les accès que ceux-ci disposent.</t>
-  </si>
-  <si>
-    <t>Seul le super administrateur peut changer les droits des administrateurs.</t>
-  </si>
-  <si>
-    <t>En tant que super administrateur, je souhaite pouvoir céder ma place à un autre administrateur afin d'octroyer les droits de super admin à un autre administrateur</t>
-  </si>
-  <si>
-    <t>Seul le super administrateur peut octroyer les droits de super admin</t>
-  </si>
-  <si>
-    <t>Il ne peut y avoir qu'un seul super admin à la fois.</t>
-  </si>
-  <si>
     <t>En tant que visiteur, je souhaite pouvoir effectuer un don afin de financer les paroisses.</t>
   </si>
   <si>
@@ -105,15 +66,6 @@
     <t>Le bouton de donation redirige vers PayPal.</t>
   </si>
   <si>
-    <t>En tant que visiteur, je souhaite pouvoir réserver des articles afin de pouvoir les récupérer lorsque je vais me rendre à la paroisse.</t>
-  </si>
-  <si>
-    <t>Il y a une notion de disponibilité des articles.</t>
-  </si>
-  <si>
-    <t>La réservation a une duré limite.</t>
-  </si>
-  <si>
     <t>En tant que visiteur, je souhaite pouvoir remplir des formulaires afin de m'inscrire aux différentes communautés religieuse</t>
   </si>
   <si>
@@ -151,6 +103,12 @@
   </si>
   <si>
     <t>Le site web a un template pour la page d'accueil avec le menu</t>
+  </si>
+  <si>
+    <t>En tant que administrateur, je souhaire pouvoir modifier les sections du sites afin de maintenir le site à jour.</t>
+  </si>
+  <si>
+    <t>Seul les administrateur peuvent modifier les section du site</t>
   </si>
 </sst>
 </file>
@@ -468,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +460,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>75</v>
@@ -511,7 +469,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -519,12 +477,12 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -533,7 +491,7 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -541,7 +499,7 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -549,12 +507,12 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -563,7 +521,7 @@
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -571,21 +529,21 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="D9">
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -593,21 +551,21 @@
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C11">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D11">
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -615,81 +573,75 @@
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>4</v>
-      </c>
-      <c r="C13">
-        <v>50</v>
-      </c>
-      <c r="D13">
+      <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>5</v>
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>30</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
       </c>
       <c r="E14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>6</v>
-      </c>
-      <c r="C15">
-        <v>5</v>
-      </c>
-      <c r="D15">
-        <v>7</v>
-      </c>
-      <c r="E15" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="B17" t="s">
         <v>7</v>
       </c>
-      <c r="C17">
-        <v>4</v>
-      </c>
-      <c r="D17">
-        <v>8</v>
-      </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>5</v>
+      <c r="A18">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>25</v>
+      </c>
+      <c r="D18">
+        <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -700,10 +652,10 @@
         <v>6</v>
       </c>
       <c r="D20">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -711,149 +663,7 @@
         <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>11</v>
-      </c>
-      <c r="C23">
-        <v>30</v>
-      </c>
-      <c r="D23">
-        <v>10</v>
-      </c>
-      <c r="E23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>10</v>
-      </c>
-      <c r="C27">
-        <v>25</v>
-      </c>
-      <c r="D27">
-        <v>11</v>
-      </c>
-      <c r="E27" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>9</v>
-      </c>
-      <c r="C29">
-        <v>15</v>
-      </c>
-      <c r="D29">
-        <v>12</v>
-      </c>
-      <c r="E29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>12</v>
-      </c>
-      <c r="C32">
-        <v>6</v>
-      </c>
-      <c r="D32">
-        <v>13</v>
-      </c>
-      <c r="E32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>5</v>
-      </c>
-      <c r="C34">
-        <v>8</v>
-      </c>
-      <c r="D34">
-        <v>14</v>
-      </c>
-      <c r="E34" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -863,10 +673,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,7 +707,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>75</v>
@@ -906,7 +716,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -914,12 +724,12 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -928,7 +738,7 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -936,7 +746,7 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -944,12 +754,12 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -958,7 +768,7 @@
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -966,29 +776,7 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <v>4</v>
-      </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fin de formulaire bénévolat
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Project-ESP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95682C89-65BA-4D7F-AD88-F7B6C8976B59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1803135F-0671-41E3-9376-D1734526B239}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -204,7 +204,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,13 +212,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -230,13 +242,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -521,7 +536,7 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
@@ -926,7 +941,7 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
@@ -1054,10 +1069,10 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
@@ -1241,7 +1256,7 @@
       <c r="D19">
         <v>8</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1249,7 +1264,7 @@
       <c r="B20" t="s">
         <v>5</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1257,7 +1272,7 @@
       <c r="B21" t="s">
         <v>6</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1265,7 +1280,7 @@
       <c r="B22" t="s">
         <v>7</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1273,7 +1288,7 @@
       <c r="B23" t="s">
         <v>35</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="1" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Version final sprint #2
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Project-ESP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1803135F-0671-41E3-9376-D1734526B239}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1526E2A-A601-437B-BEB7-7711D744C3DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="59">
   <si>
     <t>ID</t>
   </si>
@@ -188,23 +188,29 @@
     <t>Les nouvelles ont une description sommaire</t>
   </si>
   <si>
-    <t>Il est possible de modifier les images et îcônes du site</t>
-  </si>
-  <si>
     <t>Il y a 5 nouvelles d'affichées dans la page d'accueil.</t>
   </si>
   <si>
-    <t>Les nouvelles sont groupés par communauté.</t>
-  </si>
-  <si>
     <t>En tant que visiteur, je souhaite pouvoir me renseigner sur les communautés afin de me tenir au courant des nouveauté de celle-ci</t>
+  </si>
+  <si>
+    <t>Il est possible de modifier les images et icônes du site</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>Il est possible de modifier le texte des pages</t>
+  </si>
+  <si>
+    <t>Les événements du calendrier se gère (ajout, modification, suppression) directement dans les pages des paroisses.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,25 +218,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -242,16 +236,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -536,7 +527,7 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
@@ -941,7 +932,7 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
@@ -1069,10 +1060,10 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
@@ -1141,7 +1132,7 @@
         <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1165,7 +1156,7 @@
         <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1177,38 +1168,38 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>6</v>
-      </c>
-      <c r="C11">
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="C12">
         <v>30</v>
       </c>
-      <c r="D11">
-        <v>6</v>
-      </c>
-      <c r="E11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>5</v>
+      <c r="D12">
+        <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E14" t="s">
         <v>36</v>
@@ -1216,7 +1207,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="E15" t="s">
         <v>50</v>
@@ -1224,7 +1215,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E16" t="s">
         <v>51</v>
@@ -1232,7 +1223,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E17" t="s">
         <v>52</v>
@@ -1240,10 +1231,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1256,7 +1247,7 @@
       <c r="D19">
         <v>8</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1264,7 +1255,7 @@
       <c r="B20" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1272,7 +1263,7 @@
       <c r="B21" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1280,7 +1271,7 @@
       <c r="B22" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1288,7 +1279,7 @@
       <c r="B23" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>